<commit_message>
edited sql condition in carSt rp
</commit_message>
<xml_diff>
--- a/public/tmp/reportCarstatus.xlsx
+++ b/public/tmp/reportCarstatus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96">
   <si>
     <t>#</t>
   </si>
@@ -102,205 +102,187 @@
     <t>ศุภวัฒน์ หลานเด็น</t>
   </si>
   <si>
-    <t>2024-07-31</t>
+    <t>2024-09-23</t>
+  </si>
+  <si>
+    <t>กพ6164</t>
+  </si>
+  <si>
+    <t>DOLPHIN</t>
+  </si>
+  <si>
+    <t>BP81-2409-0025</t>
+  </si>
+  <si>
+    <t>M-กลาง</t>
+  </si>
+  <si>
+    <t>ทิพยประกันภัย</t>
+  </si>
+  <si>
+    <t>2024-08-26</t>
+  </si>
+  <si>
+    <t>2024-09-16</t>
+  </si>
+  <si>
+    <t>กธ-8547</t>
+  </si>
+  <si>
+    <t>Xpander</t>
+  </si>
+  <si>
+    <t>BP81-2408-0069</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>นวกิจ</t>
+  </si>
+  <si>
+    <t>สิทธิศักดิ์ กังสกุล</t>
+  </si>
+  <si>
+    <t>2024-09-06</t>
+  </si>
+  <si>
+    <t>2024-09-20</t>
+  </si>
+  <si>
+    <t>กพ4420</t>
+  </si>
+  <si>
+    <t>Triton</t>
+  </si>
+  <si>
+    <t>BP81-2409-0015</t>
+  </si>
+  <si>
+    <t>คุ้มภัยโตเกียว</t>
+  </si>
+  <si>
+    <t>2024-09-10</t>
+  </si>
+  <si>
+    <t>กพ1021</t>
+  </si>
+  <si>
+    <t>BP81-2409-0026</t>
+  </si>
+  <si>
+    <t>2024-08-31</t>
+  </si>
+  <si>
+    <t>2024-09-14</t>
+  </si>
+  <si>
+    <t>กพ9402</t>
+  </si>
+  <si>
+    <t>Mirage</t>
+  </si>
+  <si>
+    <t>BP81-2408-0097</t>
+  </si>
+  <si>
+    <t>2024-08-28</t>
+  </si>
+  <si>
+    <t>2024-09-18</t>
+  </si>
+  <si>
+    <t>8กข3121</t>
+  </si>
+  <si>
+    <t>BP81-2408-0082</t>
+  </si>
+  <si>
+    <t>BP81-2408-0083</t>
+  </si>
+  <si>
+    <t>09-09-2567 สั่งอะไหล่เพิ่มเติม (คิ้วกันชนหน้าตัวล่างขวา)</t>
+  </si>
+  <si>
+    <t>2024-09-04</t>
+  </si>
+  <si>
+    <t>2024-10-09</t>
+  </si>
+  <si>
+    <t>กบ5413</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>เมืองไทยประกัน</t>
+  </si>
+  <si>
+    <t>กน4856</t>
+  </si>
+  <si>
+    <t>BP81-2409-0023</t>
+  </si>
+  <si>
+    <t>2024-09-30</t>
+  </si>
+  <si>
+    <t>กบ209</t>
+  </si>
+  <si>
+    <t>BP81-2409-0022</t>
+  </si>
+  <si>
+    <t>10-09-2567 ขออนุมัติเพิ่มเติม (สั่งอะไหล่เพิ่มเติมฝากระบะท้าย,บานพับ,กันชนหลัง,โคลงกันชนหลัง)</t>
+  </si>
+  <si>
+    <t>4ขพ842</t>
+  </si>
+  <si>
+    <t>Jolion</t>
+  </si>
+  <si>
+    <t>BP81-2409-0029</t>
+  </si>
+  <si>
+    <t>VIN002704</t>
+  </si>
+  <si>
+    <t>BP81-2409-0019</t>
+  </si>
+  <si>
+    <t>10-9-2567 รายการอนุมัติค่าแรงเพิ่มเติม(เบ้าไฟท้าย,ซับในกระบะ)</t>
+  </si>
+  <si>
+    <t>2024-08-29</t>
   </si>
   <si>
     <t>เลยกำหนด</t>
   </si>
   <si>
-    <t>2024-09-14</t>
-  </si>
-  <si>
-    <t>กพ5077</t>
-  </si>
-  <si>
-    <t>BP81-2407-0078</t>
+    <t>2024-09-12</t>
+  </si>
+  <si>
+    <t>2ขฒ2213</t>
+  </si>
+  <si>
+    <t>BP81-2408-0091</t>
+  </si>
+  <si>
+    <t>รอเสนอตรวจเช็คกระจกมองข้างพิ่มเติม</t>
+  </si>
+  <si>
+    <t>2024-08-30</t>
+  </si>
+  <si>
+    <t>2024-10-14</t>
+  </si>
+  <si>
+    <t>BP81-2408-0096</t>
   </si>
   <si>
     <t>H3</t>
-  </si>
-  <si>
-    <t>คุ้มภัยโตเกียว</t>
-  </si>
-  <si>
-    <t>สิทธิศักดิ์ กังสกุล</t>
-  </si>
-  <si>
-    <t>2024-09-03</t>
-  </si>
-  <si>
-    <t>กง2651</t>
-  </si>
-  <si>
-    <t>Space Wagon</t>
-  </si>
-  <si>
-    <t>BP81-2409-0008</t>
-  </si>
-  <si>
-    <t>2024-09-23</t>
-  </si>
-  <si>
-    <t>กพ6164</t>
-  </si>
-  <si>
-    <t>DOLPHIN</t>
-  </si>
-  <si>
-    <t>BP81-2409-0025</t>
-  </si>
-  <si>
-    <t>M-กลาง</t>
-  </si>
-  <si>
-    <t>ทิพยประกันภัย</t>
-  </si>
-  <si>
-    <t>2024-08-26</t>
-  </si>
-  <si>
-    <t>บย501</t>
-  </si>
-  <si>
-    <t>Triton</t>
-  </si>
-  <si>
-    <t>BP81-2408-0074</t>
-  </si>
-  <si>
-    <t>นวกิจ</t>
-  </si>
-  <si>
-    <t>BP81-2408-0075</t>
-  </si>
-  <si>
-    <t>BP81-2408-0076</t>
-  </si>
-  <si>
-    <t>2024-09-16</t>
-  </si>
-  <si>
-    <t>กธ-8547</t>
-  </si>
-  <si>
-    <t>Xpander</t>
-  </si>
-  <si>
-    <t>BP81-2408-0069</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>2024-09-06</t>
-  </si>
-  <si>
-    <t>2024-09-20</t>
-  </si>
-  <si>
-    <t>กพ4420</t>
-  </si>
-  <si>
-    <t>BP81-2409-0015</t>
-  </si>
-  <si>
-    <t>2024-09-10</t>
-  </si>
-  <si>
-    <t>กพ1021</t>
-  </si>
-  <si>
-    <t>BP81-2409-0026</t>
-  </si>
-  <si>
-    <t>2024-08-31</t>
-  </si>
-  <si>
-    <t>กพ9402</t>
-  </si>
-  <si>
-    <t>Mirage</t>
-  </si>
-  <si>
-    <t>BP81-2408-0097</t>
-  </si>
-  <si>
-    <t>2024-08-28</t>
-  </si>
-  <si>
-    <t>2024-09-18</t>
-  </si>
-  <si>
-    <t>8กข3121</t>
-  </si>
-  <si>
-    <t>BP81-2408-0082</t>
-  </si>
-  <si>
-    <t>BP81-2408-0083</t>
-  </si>
-  <si>
-    <t>09-09-2567 สั่งอะไหล่เพิ่มเติม (คิ้วกันชนหน้าตัวล่างขวา)</t>
-  </si>
-  <si>
-    <t>2024-09-04</t>
-  </si>
-  <si>
-    <t>2024-10-09</t>
-  </si>
-  <si>
-    <t>กบ5413</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>เมืองไทยประกัน</t>
-  </si>
-  <si>
-    <t>กน4856</t>
-  </si>
-  <si>
-    <t>BP81-2409-0023</t>
-  </si>
-  <si>
-    <t>2024-09-30</t>
-  </si>
-  <si>
-    <t>กบ209</t>
-  </si>
-  <si>
-    <t>BP81-2409-0022</t>
-  </si>
-  <si>
-    <t>VIN002704</t>
-  </si>
-  <si>
-    <t>BP81-2409-0019</t>
-  </si>
-  <si>
-    <t>2024-08-29</t>
-  </si>
-  <si>
-    <t>2024-09-12</t>
-  </si>
-  <si>
-    <t>2ขฒ2213</t>
-  </si>
-  <si>
-    <t>BP81-2408-0091</t>
-  </si>
-  <si>
-    <t>รอเสนอตรวจเช็คกระจกมองข้างพิ่มเติม</t>
-  </si>
-  <si>
-    <t>2024-08-30</t>
-  </si>
-  <si>
-    <t>2024-10-14</t>
-  </si>
-  <si>
-    <t>BP81-2408-0096</t>
   </si>
   <si>
     <t>บย2898</t>
@@ -723,10 +705,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A2" sqref="A2:W23"/>
+      <selection activeCell="A2" sqref="A2:W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -808,7 +790,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="8">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>20</v>
@@ -857,48 +839,48 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="8">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6">
-        <v>142132.0</v>
+        <v>16607.5</v>
       </c>
       <c r="O3" s="6">
-        <v>209187.7</v>
+        <v>0.0</v>
       </c>
       <c r="P3" s="6">
-        <v>351319.7</v>
+        <v>16607.5</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
@@ -912,48 +894,48 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="8">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="H4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="L4" s="6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6">
-        <v>7260.0</v>
+        <v>44277.5</v>
       </c>
       <c r="O4" s="6">
-        <v>33442.4</v>
+        <v>53196.4</v>
       </c>
       <c r="P4" s="6">
-        <v>40702.4</v>
+        <v>97473.9</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -967,45 +949,45 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6">
-        <v>16607.5</v>
+        <v>28560.0</v>
       </c>
       <c r="O5" s="6">
-        <v>0.0</v>
+        <v>8109.0</v>
       </c>
       <c r="P5" s="6">
-        <v>16607.5</v>
+        <v>36669.0</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>27</v>
@@ -1022,48 +1004,48 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="8">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6">
-        <v>2125.0</v>
+        <v>1020.0</v>
       </c>
       <c r="O6" s="6">
-        <v>9228.45</v>
+        <v>0.0</v>
       </c>
       <c r="P6" s="6">
-        <v>11353.45</v>
+        <v>1020.0</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
@@ -1077,48 +1059,48 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="8">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="H7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6">
-        <v>15215.0</v>
+        <v>18615.0</v>
       </c>
       <c r="O7" s="6">
-        <v>5700.1</v>
+        <v>15075.69</v>
       </c>
       <c r="P7" s="6">
-        <v>20915.1</v>
+        <v>33690.69</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
@@ -1132,48 +1114,48 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="H8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6">
-        <v>14450.0</v>
+        <v>18785.0</v>
       </c>
       <c r="O8" s="6">
-        <v>277.1</v>
+        <v>260.95</v>
       </c>
       <c r="P8" s="6">
-        <v>14727.1</v>
+        <v>19045.95</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
@@ -1187,50 +1169,52 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6">
-        <v>44277.5</v>
+        <v>41820.0</v>
       </c>
       <c r="O9" s="6">
-        <v>53196.4</v>
+        <v>7595.1</v>
       </c>
       <c r="P9" s="6">
-        <v>97473.9</v>
+        <v>49415.1</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R9" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
@@ -1242,45 +1226,43 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>61</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="J10" s="6"/>
       <c r="K10" s="6" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6">
-        <v>28560.0</v>
+        <v>44767.0</v>
       </c>
       <c r="O10" s="6">
-        <v>8109.0</v>
+        <v>142349.09</v>
       </c>
       <c r="P10" s="6">
-        <v>36669.0</v>
+        <v>187116.09</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>27</v>
@@ -1297,48 +1279,48 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6">
-        <v>1020.0</v>
+        <v>8313.0</v>
       </c>
       <c r="O11" s="6">
-        <v>0.0</v>
+        <v>6920.7</v>
       </c>
       <c r="P11" s="6">
-        <v>1020.0</v>
+        <v>15233.7</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
@@ -1352,50 +1334,52 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6">
-        <v>18615.0</v>
+        <v>25372.5</v>
       </c>
       <c r="O12" s="6">
-        <v>15075.69</v>
+        <v>15928.15</v>
       </c>
       <c r="P12" s="6">
-        <v>33690.69</v>
+        <v>41300.65</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R12" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -1407,48 +1391,48 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="8">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6">
-        <v>18785.0</v>
+        <v>5770.0</v>
       </c>
       <c r="O13" s="6">
-        <v>260.95</v>
+        <v>27367.42</v>
       </c>
       <c r="P13" s="6">
-        <v>19045.95</v>
+        <v>33137.42</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
@@ -1462,51 +1446,51 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="6">
-        <v>41820.0</v>
+        <v>18785.0</v>
       </c>
       <c r="O14" s="6">
-        <v>7595.1</v>
+        <v>6747.3</v>
       </c>
       <c r="P14" s="6">
-        <v>49415.1</v>
+        <v>25532.3</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
@@ -1519,48 +1503,52 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="8">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" s="6"/>
+        <v>37</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="K15" s="6" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6">
-        <v>44767.0</v>
+        <v>25330.0</v>
       </c>
       <c r="O15" s="6">
-        <v>142349.09</v>
+        <v>13702.85</v>
       </c>
       <c r="P15" s="6">
-        <v>187116.09</v>
+        <v>39032.85</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R15" s="6"/>
+      <c r="R15" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
@@ -1572,48 +1560,48 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6">
-        <v>8313.0</v>
+        <v>8585.0</v>
       </c>
       <c r="O16" s="6">
-        <v>6920.7</v>
+        <v>511.7</v>
       </c>
       <c r="P16" s="6">
-        <v>15233.7</v>
+        <v>9096.7</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
@@ -1633,44 +1621,48 @@
         <v>19</v>
       </c>
       <c r="D17" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M17" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="N17" s="6">
-        <v>25372.5</v>
+        <v>935.0</v>
       </c>
       <c r="O17" s="6">
-        <v>15928.15</v>
+        <v>8937.85</v>
       </c>
       <c r="P17" s="6">
-        <v>41300.65</v>
+        <v>9872.85</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R17" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
@@ -1688,7 +1680,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
@@ -1698,32 +1690,32 @@
         <v>21</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6">
-        <v>12707.5</v>
+        <v>5000.0</v>
       </c>
       <c r="O18" s="6">
-        <v>6747.3</v>
+        <v>0.0</v>
       </c>
       <c r="P18" s="6">
-        <v>19454.8</v>
+        <v>5000.0</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
@@ -1733,255 +1725,29 @@
       <c r="W18" s="6"/>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="6">
-        <v>18</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="8">
-        <v>12</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6">
-        <v>25330.0</v>
-      </c>
-      <c r="O19" s="6">
-        <v>13702.85</v>
-      </c>
-      <c r="P19" s="6">
-        <v>39032.85</v>
-      </c>
-      <c r="Q19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R19" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-    </row>
-    <row r="20" spans="1:23">
-      <c r="A20" s="6">
-        <v>19</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="8">
-        <v>11</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6">
-        <v>8585.0</v>
-      </c>
-      <c r="O20" s="6">
-        <v>511.7</v>
-      </c>
-      <c r="P20" s="6">
-        <v>9096.7</v>
-      </c>
-      <c r="Q20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-    </row>
-    <row r="21" spans="1:23">
-      <c r="A21" s="6">
-        <v>20</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="8">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N21" s="6">
-        <v>935.0</v>
-      </c>
-      <c r="O21" s="6">
-        <v>8937.85</v>
-      </c>
-      <c r="P21" s="6">
-        <v>9872.85</v>
-      </c>
-      <c r="Q21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R21" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-    </row>
-    <row r="22" spans="1:23">
-      <c r="A22" s="6">
-        <v>21</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="8">
-        <v>1</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6">
-        <v>5000.0</v>
-      </c>
-      <c r="O22" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="P22" s="6">
-        <v>5000.0</v>
-      </c>
-      <c r="Q22" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
-      <c r="W22" s="6"/>
-    </row>
-    <row r="23" spans="1:23">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -1999,7 +1765,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2015,7 +1781,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2026,69 +1792,69 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2096,53 +1862,53 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>73</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
         <v>0</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2150,70 +1916,70 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20">
         <v>0</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>76</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="B22">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2221,10 +1987,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2232,57 +1998,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited car status report
</commit_message>
<xml_diff>
--- a/public/tmp/reportCarstatus.xlsx
+++ b/public/tmp/reportCarstatus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>#</t>
   </si>
@@ -72,250 +72,217 @@
     <t>หมายเหตุ</t>
   </si>
   <si>
+    <t>2024-09-11</t>
+  </si>
+  <si>
+    <t>0000-00-00</t>
+  </si>
+  <si>
+    <t>ปกติ</t>
+  </si>
+  <si>
+    <t>2024-09-17</t>
+  </si>
+  <si>
+    <t>กท3</t>
+  </si>
+  <si>
+    <t>ATTO 3</t>
+  </si>
+  <si>
+    <t>BP81-2409-0032</t>
+  </si>
+  <si>
+    <t>L-เบา</t>
+  </si>
+  <si>
+    <t>คุ้มภัยโตเกียว</t>
+  </si>
+  <si>
+    <t>ศุภวัฒน์ หลานเด็น</t>
+  </si>
+  <si>
     <t>2024-09-09</t>
   </si>
   <si>
-    <t>0000-00-00</t>
-  </si>
-  <si>
-    <t>ปกติ</t>
+    <t>2024-09-23</t>
+  </si>
+  <si>
+    <t>กพ6164</t>
+  </si>
+  <si>
+    <t>DOLPHIN</t>
+  </si>
+  <si>
+    <t>BP81-2409-0025</t>
+  </si>
+  <si>
+    <t>M-กลาง</t>
+  </si>
+  <si>
+    <t>ทิพยประกันภัย</t>
+  </si>
+  <si>
+    <t>2024-09-06</t>
+  </si>
+  <si>
+    <t>2024-09-20</t>
+  </si>
+  <si>
+    <t>กพ4420</t>
+  </si>
+  <si>
+    <t>Triton</t>
+  </si>
+  <si>
+    <t>BP81-2409-0015</t>
+  </si>
+  <si>
+    <t>2024-08-31</t>
+  </si>
+  <si>
+    <t>เลยกำหนด</t>
+  </si>
+  <si>
+    <t>2024-09-14</t>
+  </si>
+  <si>
+    <t>กพ9402</t>
+  </si>
+  <si>
+    <t>Mirage</t>
+  </si>
+  <si>
+    <t>BP81-2408-0097</t>
+  </si>
+  <si>
+    <t>สิทธิศักดิ์ กังสกุล</t>
+  </si>
+  <si>
+    <t>2024-09-04</t>
+  </si>
+  <si>
+    <t>2024-10-09</t>
+  </si>
+  <si>
+    <t>กบ5413</t>
+  </si>
+  <si>
+    <t>Xpander</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>เมืองไทยประกัน</t>
+  </si>
+  <si>
+    <t>2024-09-13</t>
+  </si>
+  <si>
+    <t>2024-09-19</t>
+  </si>
+  <si>
+    <t>กบ8862</t>
+  </si>
+  <si>
+    <t>Attrage</t>
+  </si>
+  <si>
+    <t>BP81-2409-0040</t>
+  </si>
+  <si>
+    <t>BP81-2409-0033</t>
+  </si>
+  <si>
+    <t>BP81-2409-0034</t>
   </si>
   <si>
     <t>2024-09-15</t>
   </si>
   <si>
-    <t>กธ737</t>
+    <t>กน4856</t>
   </si>
   <si>
     <t>Pajero</t>
   </si>
   <si>
-    <t>BP81-2409-0018</t>
-  </si>
-  <si>
-    <t>L-เบา</t>
-  </si>
-  <si>
-    <t>วิริยะประกันภัย</t>
-  </si>
-  <si>
-    <t>ศุภวัฒน์ หลานเด็น</t>
-  </si>
-  <si>
-    <t>2024-09-11</t>
-  </si>
-  <si>
-    <t>2024-09-17</t>
-  </si>
-  <si>
-    <t>กท3</t>
-  </si>
-  <si>
-    <t>ATTO 3</t>
-  </si>
-  <si>
-    <t>BP81-2409-0032</t>
-  </si>
-  <si>
-    <t>คุ้มภัยโตเกียว</t>
-  </si>
-  <si>
-    <t>2024-09-23</t>
-  </si>
-  <si>
-    <t>กพ6164</t>
-  </si>
-  <si>
-    <t>DOLPHIN</t>
-  </si>
-  <si>
-    <t>BP81-2409-0025</t>
-  </si>
-  <si>
-    <t>M-กลาง</t>
-  </si>
-  <si>
-    <t>ทิพยประกันภัย</t>
-  </si>
-  <si>
-    <t>2024-08-26</t>
-  </si>
-  <si>
-    <t>2024-09-16</t>
-  </si>
-  <si>
-    <t>กธ-8547</t>
-  </si>
-  <si>
-    <t>Xpander</t>
-  </si>
-  <si>
-    <t>BP81-2408-0069</t>
+    <t>BP81-2409-0023</t>
+  </si>
+  <si>
+    <t>12-09-2567 สั่งอะไหล่เพิ่มเติม (หม้อพักท่อไอเสีย)</t>
+  </si>
+  <si>
+    <t>2024-09-30</t>
+  </si>
+  <si>
+    <t>กบ209</t>
+  </si>
+  <si>
+    <t>BP81-2409-0022</t>
   </si>
   <si>
     <t>H1</t>
   </si>
   <si>
-    <t>นวกิจ</t>
-  </si>
-  <si>
-    <t>สิทธิศักดิ์ กังสกุล</t>
-  </si>
-  <si>
-    <t>2024-09-06</t>
-  </si>
-  <si>
-    <t>2024-09-20</t>
-  </si>
-  <si>
-    <t>กพ4420</t>
-  </si>
-  <si>
-    <t>Triton</t>
-  </si>
-  <si>
-    <t>BP81-2409-0015</t>
-  </si>
-  <si>
-    <t>2024-08-31</t>
-  </si>
-  <si>
-    <t>เลยกำหนด</t>
-  </si>
-  <si>
-    <t>2024-09-14</t>
-  </si>
-  <si>
-    <t>กพ9402</t>
-  </si>
-  <si>
-    <t>Mirage</t>
-  </si>
-  <si>
-    <t>BP81-2408-0097</t>
-  </si>
-  <si>
-    <t>2024-08-28</t>
+    <t>10-09-2567 ขออนุมัติเพิ่มเติม (สั่งอะไหล่เพิ่มเติมฝากระบะท้าย,บานพับ,กันชนหลัง,โคลงกันชนหลัง)</t>
+  </si>
+  <si>
+    <t>VIN002704</t>
+  </si>
+  <si>
+    <t>BP81-2409-0019</t>
+  </si>
+  <si>
+    <t>10-9-2567 รายการอนุมัติค่าแรงเพิ่มเติม(เบ้าไฟท้าย,ซับในกระบะ)</t>
+  </si>
+  <si>
+    <t>2024-08-29</t>
+  </si>
+  <si>
+    <t>2024-09-12</t>
+  </si>
+  <si>
+    <t>2ขฒ2213</t>
+  </si>
+  <si>
+    <t>BP81-2408-0091</t>
+  </si>
+  <si>
+    <t>รอเสนอตรวจเช็คกระจกมองข้างพิ่มเติม</t>
+  </si>
+  <si>
+    <t>2024-09-25</t>
+  </si>
+  <si>
+    <t>7กด4315 ( 2 )</t>
+  </si>
+  <si>
+    <t>BP81-2409-0030</t>
+  </si>
+  <si>
+    <t>12-09-2567 สั่งอะหล่เพิ่มเติม(กาบล่างกันชนหลัง)</t>
   </si>
   <si>
     <t>2024-09-18</t>
   </si>
   <si>
-    <t>8กข3121</t>
-  </si>
-  <si>
-    <t>BP81-2408-0082</t>
-  </si>
-  <si>
-    <t>BP81-2408-0083</t>
-  </si>
-  <si>
-    <t>09-09-2567 สั่งอะไหล่เพิ่มเติม (คิ้วกันชนหน้าตัวล่างขวา)</t>
-  </si>
-  <si>
-    <t>2024-09-04</t>
-  </si>
-  <si>
-    <t>2024-10-09</t>
-  </si>
-  <si>
-    <t>กบ5413</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>เมืองไทยประกัน</t>
-  </si>
-  <si>
-    <t>BP81-2409-0033</t>
-  </si>
-  <si>
-    <t>BP81-2409-0034</t>
-  </si>
-  <si>
-    <t>กน4856</t>
-  </si>
-  <si>
-    <t>BP81-2409-0023</t>
-  </si>
-  <si>
-    <t>2024-09-30</t>
-  </si>
-  <si>
-    <t>กบ209</t>
-  </si>
-  <si>
-    <t>BP81-2409-0022</t>
-  </si>
-  <si>
-    <t>10-09-2567 ขออนุมัติเพิ่มเติม (สั่งอะไหล่เพิ่มเติมฝากระบะท้าย,บานพับ,กันชนหลัง,โคลงกันชนหลัง)</t>
-  </si>
-  <si>
-    <t>2024-09-10</t>
-  </si>
-  <si>
-    <t>4ขพ842</t>
-  </si>
-  <si>
-    <t>Jolion</t>
-  </si>
-  <si>
-    <t>BP81-2409-0029</t>
-  </si>
-  <si>
-    <t>VIN002704</t>
-  </si>
-  <si>
-    <t>BP81-2409-0019</t>
-  </si>
-  <si>
-    <t>10-9-2567 รายการอนุมัติค่าแรงเพิ่มเติม(เบ้าไฟท้าย,ซับในกระบะ)</t>
-  </si>
-  <si>
-    <t>2024-08-29</t>
-  </si>
-  <si>
-    <t>2024-09-12</t>
-  </si>
-  <si>
-    <t>2ขฒ2213</t>
-  </si>
-  <si>
-    <t>BP81-2408-0091</t>
-  </si>
-  <si>
-    <t>รอเสนอตรวจเช็คกระจกมองข้างพิ่มเติม</t>
-  </si>
-  <si>
-    <t>2024-08-30</t>
-  </si>
-  <si>
-    <t>2024-10-14</t>
-  </si>
-  <si>
-    <t>BP81-2408-0096</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>2024-09-25</t>
-  </si>
-  <si>
-    <t>7กด4315 ( 2 )</t>
-  </si>
-  <si>
-    <t>BP81-2409-0030</t>
-  </si>
-  <si>
-    <t>บย2898</t>
-  </si>
-  <si>
-    <t>BP81-2409-0020</t>
-  </si>
-  <si>
-    <t>09-09-2567 ขออนุมัติรายการอะไหล่เพิ่มเติม(	กันชนเสริมหน้า)</t>
+    <t>กพ6992</t>
+  </si>
+  <si>
+    <t>BP81-2409-0035</t>
+  </si>
+  <si>
+    <t>5ขจ3562</t>
+  </si>
+  <si>
+    <t>BP81-2409-0037</t>
+  </si>
+  <si>
+    <t>9กฌ469</t>
+  </si>
+  <si>
+    <t>BP81-2409-0038</t>
   </si>
   <si>
     <t>7กด4315 ( 3 )</t>
@@ -324,22 +291,34 @@
     <t>BP81-2409-0031</t>
   </si>
   <si>
+    <t>บย1239</t>
+  </si>
+  <si>
+    <t>BP81-2409-0039</t>
+  </si>
+  <si>
+    <t>เทเวศประกันภัย</t>
+  </si>
+  <si>
+    <t>กน2315</t>
+  </si>
+  <si>
+    <t>BP81-2409-0041</t>
+  </si>
+  <si>
     <t>รายงานผลรวมของระยะเวลาการซ่อม</t>
   </si>
   <si>
-    <t>H1 (50)</t>
-  </si>
-  <si>
-    <t>H2 (8)</t>
-  </si>
-  <si>
-    <t>H3 (13)</t>
-  </si>
-  <si>
-    <t>L-เบา (28)</t>
-  </si>
-  <si>
-    <t>M-กลาง (38)</t>
+    <t>H1 (25 วัน)</t>
+  </si>
+  <si>
+    <t>H2 (35 วัน)</t>
+  </si>
+  <si>
+    <t>L-เบา (6 วัน)</t>
+  </si>
+  <si>
+    <t>M-กลาง (14 วัน)</t>
   </si>
 </sst>
 </file>
@@ -748,10 +727,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A2" sqref="A2:W22"/>
+      <selection activeCell="A2" sqref="A2:W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -859,13 +838,13 @@
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6">
-        <v>6273.0</v>
+        <v>3575.0</v>
       </c>
       <c r="O2" s="6">
         <v>0.0</v>
       </c>
       <c r="P2" s="6">
-        <v>6273.0</v>
+        <v>3575.0</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>27</v>
@@ -888,7 +867,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>20</v>
@@ -907,20 +886,20 @@
         <v>32</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6">
-        <v>3575.0</v>
+        <v>16607.5</v>
       </c>
       <c r="O3" s="6">
         <v>0.0</v>
       </c>
       <c r="P3" s="6">
-        <v>3575.0</v>
+        <v>16607.5</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>27</v>
@@ -937,45 +916,45 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6">
-        <v>16607.5</v>
+        <v>28560.0</v>
       </c>
       <c r="O4" s="6">
-        <v>0.0</v>
+        <v>8109.0</v>
       </c>
       <c r="P4" s="6">
-        <v>16607.5</v>
+        <v>36669.0</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>27</v>
@@ -998,42 +977,42 @@
         <v>19</v>
       </c>
       <c r="D5" s="8">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6">
-        <v>44277.5</v>
+        <v>18615.0</v>
       </c>
       <c r="O5" s="6">
-        <v>53196.4</v>
+        <v>15075.69</v>
       </c>
       <c r="P5" s="6">
-        <v>97473.9</v>
+        <v>33690.69</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
@@ -1047,45 +1026,43 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6"/>
+      <c r="K6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6">
-        <v>28560.0</v>
+        <v>44767.0</v>
       </c>
       <c r="O6" s="6">
-        <v>8109.0</v>
+        <v>142349.09</v>
       </c>
       <c r="P6" s="6">
-        <v>36669.0</v>
+        <v>187116.09</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>27</v>
@@ -1108,42 +1085,42 @@
         <v>19</v>
       </c>
       <c r="D7" s="8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="K7" s="6" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6">
-        <v>18615.0</v>
+        <v>8205.0</v>
       </c>
       <c r="O7" s="6">
-        <v>15075.69</v>
+        <v>8157.45</v>
       </c>
       <c r="P7" s="6">
-        <v>33690.69</v>
+        <v>16362.45</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
@@ -1157,48 +1134,48 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="8">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6">
-        <v>18785.0</v>
+        <v>6045.0</v>
       </c>
       <c r="O8" s="6">
-        <v>260.95</v>
+        <v>0.0</v>
       </c>
       <c r="P8" s="6">
-        <v>19045.95</v>
+        <v>6045.0</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
@@ -1212,52 +1189,50 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="8">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6">
-        <v>41820.0</v>
+        <v>8645.0</v>
       </c>
       <c r="O9" s="6">
-        <v>7595.1</v>
+        <v>0.0</v>
       </c>
       <c r="P9" s="6">
-        <v>49415.1</v>
+        <v>8645.0</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>64</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
@@ -1269,48 +1244,52 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="K10" s="6" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6">
-        <v>44767.0</v>
+        <v>8313.0</v>
       </c>
       <c r="O10" s="6">
-        <v>142349.09</v>
+        <v>12343.7</v>
       </c>
       <c r="P10" s="6">
-        <v>187116.09</v>
+        <v>20656.7</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R10" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
@@ -1328,44 +1307,46 @@
         <v>19</v>
       </c>
       <c r="D11" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6">
-        <v>6045.0</v>
+        <v>25372.5</v>
       </c>
       <c r="O11" s="6">
-        <v>0.0</v>
+        <v>15928.15</v>
       </c>
       <c r="P11" s="6">
-        <v>6045.0</v>
+        <v>41300.65</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R11" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -1383,7 +1364,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
@@ -1393,34 +1374,36 @@
         <v>29</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>71</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6">
-        <v>8645.0</v>
+        <v>18785.0</v>
       </c>
       <c r="O12" s="6">
-        <v>0.0</v>
+        <v>6747.3</v>
       </c>
       <c r="P12" s="6">
-        <v>8645.0</v>
+        <v>25532.3</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R12" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -1432,50 +1415,52 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="8">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6">
-        <v>8313.0</v>
+        <v>25330.0</v>
       </c>
       <c r="O13" s="6">
-        <v>6920.7</v>
+        <v>13702.85</v>
       </c>
       <c r="P13" s="6">
-        <v>15233.7</v>
+        <v>39032.85</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="R13" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
@@ -1500,38 +1485,38 @@
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="6">
-        <v>25372.5</v>
+        <v>25840.0</v>
       </c>
       <c r="O14" s="6">
-        <v>15928.15</v>
+        <v>4952.95</v>
       </c>
       <c r="P14" s="6">
-        <v>41300.65</v>
+        <v>30792.95</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
@@ -1544,7 +1529,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>19</v>
@@ -1557,35 +1542,35 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6">
-        <v>5770.0</v>
+        <v>3485.0</v>
       </c>
       <c r="O15" s="6">
-        <v>27367.42</v>
+        <v>6681.0</v>
       </c>
       <c r="P15" s="6">
-        <v>33137.42</v>
+        <v>10166.0</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
@@ -1599,52 +1584,50 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6">
-        <v>18785.0</v>
+        <v>4896.0</v>
       </c>
       <c r="O16" s="6">
-        <v>6747.3</v>
+        <v>0.0</v>
       </c>
       <c r="P16" s="6">
-        <v>25532.3</v>
+        <v>4896.0</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="R16" s="6" t="s">
-        <v>84</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="R16" s="6"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
@@ -1656,52 +1639,50 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="8">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>87</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>88</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M17" s="6"/>
       <c r="N17" s="6">
-        <v>25330.0</v>
+        <v>10795.0</v>
       </c>
       <c r="O17" s="6">
-        <v>13702.85</v>
+        <v>4715.8</v>
       </c>
       <c r="P17" s="6">
-        <v>39032.85</v>
+        <v>15510.8</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R17" s="6" t="s">
-        <v>89</v>
-      </c>
+      <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
@@ -1713,48 +1694,48 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="8">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6">
-        <v>8585.0</v>
+        <v>20485.0</v>
       </c>
       <c r="O18" s="6">
-        <v>511.7</v>
+        <v>0.0</v>
       </c>
       <c r="P18" s="6">
-        <v>9096.7</v>
+        <v>20485.0</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
@@ -1768,7 +1749,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>19</v>
@@ -1781,35 +1762,35 @@
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="M19" s="6"/>
       <c r="N19" s="6">
-        <v>27285.0</v>
+        <v>6502.5</v>
       </c>
       <c r="O19" s="6">
-        <v>4043.45</v>
+        <v>5609.24</v>
       </c>
       <c r="P19" s="6">
-        <v>31328.45</v>
+        <v>12111.74</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
@@ -1823,54 +1804,50 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6">
+        <v>3672.0</v>
+      </c>
+      <c r="O20" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="P20" s="6">
+        <v>3672.0</v>
+      </c>
+      <c r="Q20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="M20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N20" s="6">
-        <v>935.0</v>
-      </c>
-      <c r="O20" s="6">
-        <v>8937.85</v>
-      </c>
-      <c r="P20" s="6">
-        <v>9872.85</v>
-      </c>
-      <c r="Q20" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="R20" s="6" t="s">
-        <v>99</v>
-      </c>
+      <c r="R20" s="6"/>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
@@ -1878,84 +1855,29 @@
       <c r="W20" s="6"/>
     </row>
     <row r="21" spans="1:23">
-      <c r="A21" s="6">
-        <v>20</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="8">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6">
-        <v>20485.0</v>
-      </c>
-      <c r="O21" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="P21" s="6">
-        <v>20485.0</v>
-      </c>
-      <c r="Q21" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-    </row>
-    <row r="22" spans="1:23">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -1973,10 +1895,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A20" sqref="A20:C20"/>
+      <selection activeCell="A18" sqref="A18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1989,7 +1911,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2000,128 +1922,132 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>15</v>
-      </c>
+      <c r="A5" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>17</v>
-      </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+      <c r="C8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
         <v>0</v>
       </c>
-      <c r="C11">
-        <v>13</v>
-      </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2132,61 +2058,61 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
+      <c r="A18" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
         <v>0</v>
       </c>
-      <c r="C19">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
+      <c r="C20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B21">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2194,21 +2120,21 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2216,46 +2142,24 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
         <v>0</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26">
-        <v>3</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add higtlight overade due
</commit_message>
<xml_diff>
--- a/public/tmp/reportCarstatus.xlsx
+++ b/public/tmp/reportCarstatus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
   <si>
     <t>#</t>
   </si>
@@ -198,64 +198,43 @@
     <t>BP81-2409-0034</t>
   </si>
   <si>
-    <t>2024-09-15</t>
-  </si>
-  <si>
-    <t>กน4856</t>
+    <t>2024-09-30</t>
+  </si>
+  <si>
+    <t>กบ209</t>
+  </si>
+  <si>
+    <t>BP81-2409-0022</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>10-09-2567 ขออนุมัติเพิ่มเติม (สั่งอะไหล่เพิ่มเติมฝากระบะท้าย,บานพับ,กันชนหลัง,โคลงกันชนหลัง)</t>
+  </si>
+  <si>
+    <t>2024-08-29</t>
+  </si>
+  <si>
+    <t>2024-09-12</t>
+  </si>
+  <si>
+    <t>2ขฒ2213</t>
+  </si>
+  <si>
+    <t>BP81-2408-0091</t>
+  </si>
+  <si>
+    <t>รอเสนอตรวจเช็คกระจกมองข้างพิ่มเติม</t>
+  </si>
+  <si>
+    <t>2024-09-25</t>
+  </si>
+  <si>
+    <t>7กด4315 ( 2 )</t>
   </si>
   <si>
     <t>Pajero</t>
-  </si>
-  <si>
-    <t>BP81-2409-0023</t>
-  </si>
-  <si>
-    <t>12-09-2567 สั่งอะไหล่เพิ่มเติม (หม้อพักท่อไอเสีย)</t>
-  </si>
-  <si>
-    <t>2024-09-30</t>
-  </si>
-  <si>
-    <t>กบ209</t>
-  </si>
-  <si>
-    <t>BP81-2409-0022</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>10-09-2567 ขออนุมัติเพิ่มเติม (สั่งอะไหล่เพิ่มเติมฝากระบะท้าย,บานพับ,กันชนหลัง,โคลงกันชนหลัง)</t>
-  </si>
-  <si>
-    <t>VIN002704</t>
-  </si>
-  <si>
-    <t>BP81-2409-0019</t>
-  </si>
-  <si>
-    <t>10-9-2567 รายการอนุมัติค่าแรงเพิ่มเติม(เบ้าไฟท้าย,ซับในกระบะ)</t>
-  </si>
-  <si>
-    <t>2024-08-29</t>
-  </si>
-  <si>
-    <t>2024-09-12</t>
-  </si>
-  <si>
-    <t>2ขฒ2213</t>
-  </si>
-  <si>
-    <t>BP81-2408-0091</t>
-  </si>
-  <si>
-    <t>รอเสนอตรวจเช็คกระจกมองข้างพิ่มเติม</t>
-  </si>
-  <si>
-    <t>2024-09-25</t>
-  </si>
-  <si>
-    <t>7กด4315 ( 2 )</t>
   </si>
   <si>
     <t>BP81-2409-0030</t>
@@ -367,7 +346,7 @@
       <name val="Candara"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +359,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFffb703"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFe85d04"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -396,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -428,6 +413,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,10 +713,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A2" sqref="A2:W21"/>
+      <selection activeCell="A2" sqref="A2:W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1263,26 +1249,26 @@
         <v>61</v>
       </c>
       <c r="I10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="K10" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6">
-        <v>8313.0</v>
+        <v>25372.5</v>
       </c>
       <c r="O10" s="6">
-        <v>12343.7</v>
+        <v>15928.15</v>
       </c>
       <c r="P10" s="6">
-        <v>20656.7</v>
+        <v>41300.65</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>46</v>
@@ -1301,48 +1287,48 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="8">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>26</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6">
-        <v>25372.5</v>
+        <v>25330.0</v>
       </c>
       <c r="O11" s="6">
-        <v>15928.15</v>
+        <v>13702.85</v>
       </c>
       <c r="P11" s="6">
-        <v>41300.65</v>
+        <v>39032.85</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="R11" s="6" t="s">
         <v>69</v>
@@ -1358,29 +1344,29 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>33</v>
@@ -1390,19 +1376,19 @@
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6">
-        <v>18785.0</v>
+        <v>25840.0</v>
       </c>
       <c r="O12" s="6">
-        <v>6747.3</v>
+        <v>4952.95</v>
       </c>
       <c r="P12" s="6">
-        <v>25532.3</v>
+        <v>30792.95</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
@@ -1415,52 +1401,50 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="8">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>50</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>26</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6">
-        <v>25330.0</v>
+        <v>3485.0</v>
       </c>
       <c r="O13" s="6">
-        <v>13702.85</v>
+        <v>6681.0</v>
       </c>
       <c r="P13" s="6">
-        <v>39032.85</v>
+        <v>10166.0</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>77</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="R13" s="6"/>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
@@ -1472,52 +1456,50 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="I14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="K14" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>26</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="6">
-        <v>25840.0</v>
+        <v>4896.0</v>
       </c>
       <c r="O14" s="6">
-        <v>4952.95</v>
+        <v>0.0</v>
       </c>
       <c r="P14" s="6">
-        <v>30792.95</v>
+        <v>4896.0</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>81</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="R14" s="6"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
@@ -1529,7 +1511,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>19</v>
@@ -1542,16 +1524,16 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>25</v>
@@ -1561,16 +1543,16 @@
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6">
-        <v>3485.0</v>
+        <v>10795.0</v>
       </c>
       <c r="O15" s="6">
-        <v>6681.0</v>
+        <v>4715.8</v>
       </c>
       <c r="P15" s="6">
-        <v>10166.0</v>
+        <v>15510.8</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
@@ -1584,48 +1566,48 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="I16" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>26</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6">
-        <v>4896.0</v>
+        <v>20485.0</v>
       </c>
       <c r="O16" s="6">
         <v>0.0</v>
       </c>
       <c r="P16" s="6">
-        <v>4896.0</v>
+        <v>20485.0</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
@@ -1639,48 +1621,48 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="M17" s="6"/>
       <c r="N17" s="6">
-        <v>10795.0</v>
+        <v>6502.5</v>
       </c>
       <c r="O17" s="6">
-        <v>4715.8</v>
+        <v>5609.24</v>
       </c>
       <c r="P17" s="6">
-        <v>15510.8</v>
+        <v>12111.74</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
@@ -1694,48 +1676,48 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>26</v>
       </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6">
-        <v>20485.0</v>
+        <v>3672.0</v>
       </c>
       <c r="O18" s="6">
         <v>0.0</v>
       </c>
       <c r="P18" s="6">
-        <v>20485.0</v>
+        <v>3672.0</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
@@ -1745,139 +1727,29 @@
       <c r="W18" s="6"/>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="6">
-        <v>18</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="8">
-        <v>1</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6">
-        <v>6502.5</v>
-      </c>
-      <c r="O19" s="6">
-        <v>5609.24</v>
-      </c>
-      <c r="P19" s="6">
-        <v>12111.74</v>
-      </c>
-      <c r="Q19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-    </row>
-    <row r="20" spans="1:23">
-      <c r="A20" s="6">
-        <v>19</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="8">
-        <v>1</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6">
-        <v>3672.0</v>
-      </c>
-      <c r="O20" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="P20" s="6">
-        <v>3672.0</v>
-      </c>
-      <c r="Q20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-    </row>
-    <row r="21" spans="1:23">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -1895,7 +1767,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A18" sqref="A18:C18"/>
@@ -1911,7 +1783,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1927,14 +1799,14 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="12" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1945,7 +1817,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="12" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -1963,14 +1835,14 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1981,7 +1853,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2025,7 +1897,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2036,61 +1908,61 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
         <v>0</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="13">
+        <v>16</v>
+      </c>
+      <c r="C18" s="13">
         <v>0</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B19">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2098,7 +1970,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -2109,10 +1981,10 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2120,45 +1992,23 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
         <v>0</v>
-      </c>
-      <c r="C22">
-        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
editing: count date delay in car status report
</commit_message>
<xml_diff>
--- a/public/tmp/reportCarstatus.xlsx
+++ b/public/tmp/reportCarstatus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
   <si>
     <t>#</t>
   </si>
@@ -72,7 +72,7 @@
     <t>หมายเหตุ</t>
   </si>
   <si>
-    <t>2024-09-11</t>
+    <t>2024-10-19</t>
   </si>
   <si>
     <t>0000-00-00</t>
@@ -81,16 +81,16 @@
     <t>ปกติ</t>
   </si>
   <si>
-    <t>2024-09-17</t>
-  </si>
-  <si>
-    <t>กท3</t>
-  </si>
-  <si>
-    <t>ATTO 3</t>
-  </si>
-  <si>
-    <t>BP81-2409-0032</t>
+    <t>2024-10-25</t>
+  </si>
+  <si>
+    <t>กพ5764</t>
+  </si>
+  <si>
+    <t>Triton</t>
+  </si>
+  <si>
+    <t>BP81-2410-0060</t>
   </si>
   <si>
     <t>L-เบา</t>
@@ -102,187 +102,247 @@
     <t>ศุภวัฒน์ หลานเด็น</t>
   </si>
   <si>
-    <t>2024-09-09</t>
-  </si>
-  <si>
-    <t>2024-09-23</t>
-  </si>
-  <si>
-    <t>กพ6164</t>
+    <t>12-09-2567 สั่งสติ๊กเกอร์ประตูหน้าซ้าย ( S-SPORTY)</t>
+  </si>
+  <si>
+    <t>2024-10-07</t>
+  </si>
+  <si>
+    <t>2024-11-21</t>
+  </si>
+  <si>
+    <t>กพ5227</t>
+  </si>
+  <si>
+    <t>Attrage</t>
+  </si>
+  <si>
+    <t>BP81-2410-0015</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>2024-10-16</t>
+  </si>
+  <si>
+    <t>2024-10-22</t>
+  </si>
+  <si>
+    <t>กท1946</t>
+  </si>
+  <si>
+    <t>BP81-2410-0049</t>
+  </si>
+  <si>
+    <t>วิริยะประกันภัย</t>
+  </si>
+  <si>
+    <t>2024-10-30</t>
+  </si>
+  <si>
+    <t>BP81-2410-0050</t>
+  </si>
+  <si>
+    <t>M-กลาง</t>
+  </si>
+  <si>
+    <t>2024-10-03</t>
+  </si>
+  <si>
+    <t>2024-10-24</t>
+  </si>
+  <si>
+    <t>3ขณ6203</t>
+  </si>
+  <si>
+    <t>Xpander</t>
+  </si>
+  <si>
+    <t>BP81-2410-0004</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>2024-10-14</t>
+  </si>
+  <si>
+    <t>2024-10-20</t>
+  </si>
+  <si>
+    <t>กท7926</t>
+  </si>
+  <si>
+    <t>Mirage</t>
+  </si>
+  <si>
+    <t>BP81-2410-0032</t>
+  </si>
+  <si>
+    <t>สิทธิศักดิ์ กังสกุล</t>
+  </si>
+  <si>
+    <t>2024-10-09</t>
+  </si>
+  <si>
+    <t>2024-11-13</t>
+  </si>
+  <si>
+    <t>9กฌ469</t>
+  </si>
+  <si>
+    <t>Pajero</t>
+  </si>
+  <si>
+    <t>BP81-2410-0020</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>12-10-2567 สั่งรายการอะไหล่เพิ่มเติม 3 รายการ(	ซับในแผงข้างขวา,แผงต่อมุมกระบะข้างด้านในขวา,คานขวางพื้นหลังขวา)</t>
+  </si>
+  <si>
+    <t>2024-10-08</t>
+  </si>
+  <si>
+    <t>กบ8595</t>
+  </si>
+  <si>
+    <t>BP81-2410-0018</t>
+  </si>
+  <si>
+    <t>2024-10-11</t>
+  </si>
+  <si>
+    <t>เลยกำหนด</t>
+  </si>
+  <si>
+    <t>2024-10-17</t>
+  </si>
+  <si>
+    <t>กค9779</t>
+  </si>
+  <si>
+    <t>CLS250 CGI2.2</t>
+  </si>
+  <si>
+    <t>BP81-2410-0027</t>
+  </si>
+  <si>
+    <t>อลิอันซ์ อยุธยา</t>
+  </si>
+  <si>
+    <t>2024-10-31</t>
+  </si>
+  <si>
+    <t>9กข3633</t>
+  </si>
+  <si>
+    <t>BP81-2410-0053</t>
+  </si>
+  <si>
+    <t>กรุงเทพประกันภัย</t>
+  </si>
+  <si>
+    <t>2024-10-15</t>
+  </si>
+  <si>
+    <t>2024-10-29</t>
+  </si>
+  <si>
+    <t>กธ6446</t>
+  </si>
+  <si>
+    <t>BP81-2410-0039</t>
+  </si>
+  <si>
+    <t>17-10-2567 สั่งอะไหล่เพิ่มเติม(ขายึดมุมกันชนขวา,บังลมหม้อน้ำ)</t>
+  </si>
+  <si>
+    <t>2024-10-21</t>
+  </si>
+  <si>
+    <t>กพ7027</t>
   </si>
   <si>
     <t>DOLPHIN</t>
   </si>
   <si>
-    <t>BP81-2409-0025</t>
-  </si>
-  <si>
-    <t>M-กลาง</t>
+    <t>BP81-2410-0041</t>
   </si>
   <si>
     <t>ทิพยประกันภัย</t>
   </si>
   <si>
-    <t>2024-09-06</t>
-  </si>
-  <si>
-    <t>2024-09-20</t>
-  </si>
-  <si>
-    <t>กพ4420</t>
-  </si>
-  <si>
-    <t>Triton</t>
-  </si>
-  <si>
-    <t>BP81-2409-0015</t>
-  </si>
-  <si>
-    <t>2024-08-31</t>
-  </si>
-  <si>
-    <t>เลยกำหนด</t>
-  </si>
-  <si>
-    <t>2024-09-14</t>
-  </si>
-  <si>
-    <t>กพ9402</t>
-  </si>
-  <si>
-    <t>Mirage</t>
-  </si>
-  <si>
-    <t>BP81-2408-0097</t>
-  </si>
-  <si>
-    <t>สิทธิศักดิ์ กังสกุล</t>
-  </si>
-  <si>
-    <t>2024-09-04</t>
-  </si>
-  <si>
-    <t>2024-10-09</t>
+    <t>บย5530</t>
+  </si>
+  <si>
+    <t>Dmax</t>
+  </si>
+  <si>
+    <t>BP81-2410-0048</t>
+  </si>
+  <si>
+    <t>นวกิจ</t>
+  </si>
+  <si>
+    <t>กน8752</t>
+  </si>
+  <si>
+    <t>BP81-2410-0045</t>
+  </si>
+  <si>
+    <t>กร6243</t>
+  </si>
+  <si>
+    <t>BP81-2410-0046</t>
+  </si>
+  <si>
+    <t>BP81-2410-0047</t>
+  </si>
+  <si>
+    <t>2024-10-23</t>
+  </si>
+  <si>
+    <t>5ขภ3418</t>
+  </si>
+  <si>
+    <t>BP81-2410-0051</t>
+  </si>
+  <si>
+    <t>BP81-2410-0052</t>
+  </si>
+  <si>
+    <t>ก2589</t>
+  </si>
+  <si>
+    <t>Goodcat</t>
+  </si>
+  <si>
+    <t>BP81-2410-0044</t>
+  </si>
+  <si>
+    <t>3ฒว9178</t>
+  </si>
+  <si>
+    <t>BP81-2410-0059</t>
+  </si>
+  <si>
+    <t>2024-10-18</t>
   </si>
   <si>
     <t>กบ5413</t>
   </si>
   <si>
-    <t>Xpander</t>
-  </si>
-  <si>
-    <t>H2</t>
+    <t>BP81-2410-0056</t>
   </si>
   <si>
     <t>เมืองไทยประกัน</t>
   </si>
   <si>
-    <t>2024-09-13</t>
-  </si>
-  <si>
-    <t>2024-09-19</t>
-  </si>
-  <si>
-    <t>กบ8862</t>
-  </si>
-  <si>
-    <t>Attrage</t>
-  </si>
-  <si>
-    <t>BP81-2409-0040</t>
-  </si>
-  <si>
-    <t>BP81-2409-0033</t>
-  </si>
-  <si>
-    <t>BP81-2409-0034</t>
-  </si>
-  <si>
-    <t>2024-09-30</t>
-  </si>
-  <si>
-    <t>กบ209</t>
-  </si>
-  <si>
-    <t>BP81-2409-0022</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>10-09-2567 ขออนุมัติเพิ่มเติม (สั่งอะไหล่เพิ่มเติมฝากระบะท้าย,บานพับ,กันชนหลัง,โคลงกันชนหลัง)</t>
-  </si>
-  <si>
-    <t>2024-08-29</t>
-  </si>
-  <si>
-    <t>2024-09-12</t>
-  </si>
-  <si>
-    <t>2ขฒ2213</t>
-  </si>
-  <si>
-    <t>BP81-2408-0091</t>
-  </si>
-  <si>
-    <t>รอเสนอตรวจเช็คกระจกมองข้างพิ่มเติม</t>
-  </si>
-  <si>
-    <t>2024-09-25</t>
-  </si>
-  <si>
-    <t>7กด4315 ( 2 )</t>
-  </si>
-  <si>
-    <t>Pajero</t>
-  </si>
-  <si>
-    <t>BP81-2409-0030</t>
-  </si>
-  <si>
-    <t>12-09-2567 สั่งอะหล่เพิ่มเติม(กาบล่างกันชนหลัง)</t>
-  </si>
-  <si>
-    <t>2024-09-18</t>
-  </si>
-  <si>
-    <t>กพ6992</t>
-  </si>
-  <si>
-    <t>BP81-2409-0035</t>
-  </si>
-  <si>
-    <t>5ขจ3562</t>
-  </si>
-  <si>
-    <t>BP81-2409-0037</t>
-  </si>
-  <si>
-    <t>9กฌ469</t>
-  </si>
-  <si>
-    <t>BP81-2409-0038</t>
-  </si>
-  <si>
-    <t>7กด4315 ( 3 )</t>
-  </si>
-  <si>
-    <t>BP81-2409-0031</t>
-  </si>
-  <si>
-    <t>บย1239</t>
-  </si>
-  <si>
-    <t>BP81-2409-0039</t>
-  </si>
-  <si>
-    <t>เทเวศประกันภัย</t>
-  </si>
-  <si>
-    <t>กน2315</t>
-  </si>
-  <si>
-    <t>BP81-2409-0041</t>
+    <t>BP81-2410-0057</t>
   </si>
   <si>
     <t>รายงานผลรวมของระยะเวลาการซ่อม</t>
@@ -292,6 +352,9 @@
   </si>
   <si>
     <t>H2 (35 วัน)</t>
+  </si>
+  <si>
+    <t>H3 (45 วัน)</t>
   </si>
   <si>
     <t>L-เบา (6 วัน)</t>
@@ -713,10 +776,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A2" sqref="A2:W19"/>
+      <selection activeCell="A2" sqref="A2:W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -798,7 +861,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>20</v>
@@ -824,18 +887,20 @@
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6">
-        <v>3575.0</v>
+        <v>9860.0</v>
       </c>
       <c r="O2" s="6">
-        <v>0.0</v>
+        <v>11955.25</v>
       </c>
       <c r="P2" s="6">
-        <v>3575.0</v>
+        <v>21815.25</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="6"/>
+      <c r="R2" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
@@ -847,45 +912,45 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="8">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6">
-        <v>16607.5</v>
+        <v>49305.0</v>
       </c>
       <c r="O3" s="6">
-        <v>0.0</v>
+        <v>219168.69</v>
       </c>
       <c r="P3" s="6">
-        <v>16607.5</v>
+        <v>268473.69</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>27</v>
@@ -908,7 +973,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>20</v>
@@ -921,26 +986,26 @@
         <v>37</v>
       </c>
       <c r="I4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6">
-        <v>28560.0</v>
+        <v>3436.0</v>
       </c>
       <c r="O4" s="6">
-        <v>8109.0</v>
+        <v>3970.0</v>
       </c>
       <c r="P4" s="6">
-        <v>36669.0</v>
+        <v>7406.0</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>27</v>
@@ -957,48 +1022,48 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="8">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="L5" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6">
-        <v>18615.0</v>
+        <v>11433.0</v>
       </c>
       <c r="O5" s="6">
-        <v>15075.69</v>
+        <v>0.0</v>
       </c>
       <c r="P5" s="6">
-        <v>33690.69</v>
+        <v>11433.0</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
@@ -1012,43 +1077,45 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="8">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="L6" s="6" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6">
-        <v>44767.0</v>
+        <v>38007.5</v>
       </c>
       <c r="O6" s="6">
-        <v>142349.09</v>
+        <v>75129.89</v>
       </c>
       <c r="P6" s="6">
-        <v>187116.09</v>
+        <v>113137.39</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>27</v>
@@ -1065,29 +1132,29 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>25</v>
@@ -1097,16 +1164,16 @@
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6">
-        <v>8205.0</v>
+        <v>11135.0</v>
       </c>
       <c r="O7" s="6">
-        <v>8157.45</v>
+        <v>2677.5</v>
       </c>
       <c r="P7" s="6">
-        <v>16362.45</v>
+        <v>13812.5</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
@@ -1120,50 +1187,52 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>26</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6">
-        <v>6045.0</v>
+        <v>33405.0</v>
       </c>
       <c r="O8" s="6">
-        <v>0.0</v>
+        <v>95239.95</v>
       </c>
       <c r="P8" s="6">
-        <v>6045.0</v>
+        <v>128644.95</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="6"/>
+      <c r="R8" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
@@ -1175,48 +1244,48 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="8">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6">
-        <v>8645.0</v>
+        <v>27489.0</v>
       </c>
       <c r="O9" s="6">
-        <v>0.0</v>
+        <v>43103.5</v>
       </c>
       <c r="P9" s="6">
-        <v>8645.0</v>
+        <v>70592.5</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
@@ -1230,52 +1299,50 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6">
-        <v>25372.5</v>
+        <v>2500.0</v>
       </c>
       <c r="O10" s="6">
-        <v>15928.15</v>
+        <v>0.0</v>
       </c>
       <c r="P10" s="6">
-        <v>41300.65</v>
+        <v>2500.0</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>64</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
@@ -1287,52 +1354,50 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="8">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6">
-        <v>25330.0</v>
+        <v>28645.0</v>
       </c>
       <c r="O11" s="6">
-        <v>13702.85</v>
+        <v>3396.4</v>
       </c>
       <c r="P11" s="6">
-        <v>39032.85</v>
+        <v>32041.4</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R11" s="6" t="s">
-        <v>69</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -1344,51 +1409,51 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6">
-        <v>25840.0</v>
+        <v>15725.0</v>
       </c>
       <c r="O12" s="6">
-        <v>4952.95</v>
+        <v>39004.45</v>
       </c>
       <c r="P12" s="6">
-        <v>30792.95</v>
+        <v>54729.45</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>27</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
@@ -1401,48 +1466,48 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6">
-        <v>3485.0</v>
+        <v>9880.0</v>
       </c>
       <c r="O13" s="6">
-        <v>6681.0</v>
+        <v>0.0</v>
       </c>
       <c r="P13" s="6">
-        <v>10166.0</v>
+        <v>9880.0</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
@@ -1456,48 +1521,48 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="6">
-        <v>4896.0</v>
+        <v>7210.0</v>
       </c>
       <c r="O14" s="6">
         <v>0.0</v>
       </c>
       <c r="P14" s="6">
-        <v>4896.0</v>
+        <v>7210.0</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
@@ -1511,29 +1576,29 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>25</v>
@@ -1543,16 +1608,16 @@
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6">
-        <v>10795.0</v>
+        <v>8704.0</v>
       </c>
       <c r="O15" s="6">
-        <v>4715.8</v>
+        <v>4115.7</v>
       </c>
       <c r="P15" s="6">
-        <v>15510.8</v>
+        <v>12819.7</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
@@ -1566,7 +1631,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>19</v>
@@ -1579,35 +1644,35 @@
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>26</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6">
-        <v>20485.0</v>
+        <v>3000.0</v>
       </c>
       <c r="O16" s="6">
-        <v>0.0</v>
+        <v>2834.75</v>
       </c>
       <c r="P16" s="6">
-        <v>20485.0</v>
+        <v>5834.75</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
@@ -1621,48 +1686,48 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="M17" s="6"/>
       <c r="N17" s="6">
-        <v>6502.5</v>
+        <v>400.0</v>
       </c>
       <c r="O17" s="6">
-        <v>5609.24</v>
+        <v>1922.7</v>
       </c>
       <c r="P17" s="6">
-        <v>12111.74</v>
+        <v>2322.7</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
@@ -1676,29 +1741,29 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>25</v>
@@ -1708,16 +1773,16 @@
       </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6">
-        <v>3672.0</v>
+        <v>11611.0</v>
       </c>
       <c r="O18" s="6">
-        <v>0.0</v>
+        <v>2929.95</v>
       </c>
       <c r="P18" s="6">
-        <v>3672.0</v>
+        <v>14540.95</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
@@ -1727,29 +1792,304 @@
       <c r="W18" s="6"/>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="8">
+        <v>2</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6">
+        <v>6494.0</v>
+      </c>
+      <c r="O19" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="P19" s="6">
+        <v>6494.0</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="8">
+        <v>3</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6">
+        <v>4930.0</v>
+      </c>
+      <c r="O20" s="6">
+        <v>18560.94</v>
+      </c>
+      <c r="P20" s="6">
+        <v>23490.94</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6">
+        <v>186.0</v>
+      </c>
+      <c r="O21" s="6">
+        <v>2550.0</v>
+      </c>
+      <c r="P21" s="6">
+        <v>2736.0</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6">
+        <v>10030.0</v>
+      </c>
+      <c r="O22" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="P22" s="6">
+        <v>10030.0</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6">
+        <v>8415.0</v>
+      </c>
+      <c r="O23" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="P23" s="6">
+        <v>8415.0</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -1767,10 +2107,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A18" sqref="A18:C18"/>
+      <selection activeCell="A25" sqref="A25:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1783,7 +2123,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1794,40 +2134,40 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="12" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="12" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1835,134 +2175,134 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="12" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
+      <c r="A9" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
         <v>3</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
         <v>3</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
+      <c r="A14" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="13">
+        <v>9</v>
+      </c>
+      <c r="C14" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="13">
-        <v>16</v>
-      </c>
-      <c r="C18" s="13">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1970,10 +2310,10 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1981,10 +2321,10 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1992,24 +2332,86 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>14</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>